<commit_message>
add another test run (this one was broken after one hour
</commit_message>
<xml_diff>
--- a/examples/test-runs/phase1-xlsx/run-20250128-203002.xlsx
+++ b/examples/test-runs/phase1-xlsx/run-20250128-203002.xlsx
@@ -2561,6 +2561,7 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2605,20 +2606,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2626,7 +2619,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2824,363 +2821,363 @@
   </sheetPr>
   <dimension ref="A1:AM46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AC28" activeCellId="0" sqref="AC28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="AD1" activeCellId="0" sqref="AD1"/>
+      <selection pane="bottomLeft" activeCell="AJ9" activeCellId="0" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="15" min="2" style="0" width="8.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="25.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="28.38"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="18" style="0" width="8.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="79.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="17.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="20.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="18.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="32" style="0" width="17.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="15.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="16.13"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="15" min="2" style="1" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="25.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="28.38"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="18" style="1" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="79.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="20.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="32" style="1" width="17.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="15.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="16.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="0" t="s">
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AG1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AI1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AK1" s="0" t="s">
+      <c r="AK1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AL1" s="0" t="s">
+      <c r="AL1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AM1" s="0" t="s">
+      <c r="AM1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="0" t="s">
+      <c r="AB2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AK2" s="0" t="s">
+      <c r="AK2" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="0" t="s">
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="S3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="T3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="U3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="V3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="W3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="X3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="Y3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="Z3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="0" t="s">
+      <c r="AA3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AB3" s="0" t="s">
+      <c r="AB3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AC3" s="0" t="s">
+      <c r="AC3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="0" t="s">
+      <c r="AD3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AE3" s="0" t="s">
+      <c r="AE3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AF3" s="0" t="s">
+      <c r="AF3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AG3" s="0" t="s">
+      <c r="AG3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AH3" s="0" t="s">
+      <c r="AH3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AI3" s="0" t="s">
+      <c r="AI3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AJ3" s="0" t="s">
+      <c r="AJ3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AK3" s="0" t="s">
+      <c r="AK3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="0" t="s">
+      <c r="AL3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AM3" s="0" t="s">
+      <c r="AM3" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="594.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>9.651055</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>1420</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>575</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>448</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="G4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>82.359094</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4" s="1" t="n">
         <v>1286</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="1" t="n">
         <v>1291</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <v>1088</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="O4" s="1" t="n">
         <v>1152</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="P4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="R4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S4" s="0" t="n">
+      <c r="S4" s="1" t="n">
         <v>13.273923</v>
       </c>
-      <c r="T4" s="0" t="n">
+      <c r="T4" s="1" t="n">
         <v>3971</v>
       </c>
-      <c r="U4" s="0" t="n">
+      <c r="U4" s="1" t="n">
         <v>581</v>
       </c>
-      <c r="V4" s="0" t="n">
+      <c r="V4" s="1" t="n">
         <v>1152</v>
       </c>
-      <c r="W4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" s="0" t="n">
+      <c r="W4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Y4" s="2" t="b">
+      <c r="Y4" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z4" s="0" t="s">
+      <c r="Z4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AA4" s="2" t="s">
         <v>37</v>
       </c>
       <c r="AB4" s="3" t="s">
@@ -3193,2479 +3190,2479 @@
       <c r="AI4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AJ4" s="4" t="s">
+      <c r="AJ4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AK4" s="2" t="b">
+      <c r="AK4" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL4" s="0" t="s">
+      <c r="AL4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AM4" s="0" t="s">
+      <c r="AM4" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" customFormat="false" ht="986.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>11.01377</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>3838</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>1252</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>1024</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="G5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="1" t="n">
         <v>76.008932</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5" s="1" t="n">
         <v>1388</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="M5" s="1" t="n">
         <v>1734</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5" s="1" t="n">
         <v>1600</v>
       </c>
-      <c r="O5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="0" t="s">
+      <c r="O5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="Q5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="R5" s="0" t="n">
+      <c r="R5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="S5" s="0" t="n">
+      <c r="S5" s="1" t="n">
         <v>21.935558</v>
       </c>
-      <c r="T5" s="0" t="n">
+      <c r="T5" s="1" t="n">
         <v>11320</v>
       </c>
-      <c r="U5" s="0" t="n">
+      <c r="U5" s="1" t="n">
         <v>995</v>
       </c>
-      <c r="V5" s="0" t="n">
+      <c r="V5" s="1" t="n">
         <v>8576</v>
       </c>
-      <c r="W5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X5" s="0" t="n">
+      <c r="W5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="Y5" s="2" t="b">
+      <c r="Y5" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Z5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AA5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AB5" s="0" t="s">
+      <c r="AB5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC5" s="0" t="s">
+      <c r="AC5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AF5" s="0" t="s">
+      <c r="AF5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AH5" s="0" t="n">
+      <c r="AH5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AI5" s="0" t="s">
+      <c r="AI5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ5" s="0" t="s">
+      <c r="AJ5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AK5" s="2" t="b">
+      <c r="AK5" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL5" s="0" t="s">
+      <c r="AL5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM5" s="0" t="s">
+      <c r="AM5" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="1894" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>17.899119</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>3565</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>1417</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>1024</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="G6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>75.05872</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6" s="1" t="n">
         <v>1545</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M6" s="1" t="n">
         <v>1610</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6" s="1" t="n">
         <v>1408</v>
       </c>
-      <c r="O6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" s="0" t="s">
+      <c r="O6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="Q6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="R6" s="0" t="n">
+      <c r="R6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="S6" s="0" t="n">
+      <c r="S6" s="1" t="n">
         <v>8.845643</v>
       </c>
-      <c r="T6" s="0" t="n">
+      <c r="T6" s="1" t="n">
         <v>6038</v>
       </c>
-      <c r="U6" s="0" t="n">
+      <c r="U6" s="1" t="n">
         <v>354</v>
       </c>
-      <c r="V6" s="0" t="n">
+      <c r="V6" s="1" t="n">
         <v>3968</v>
       </c>
-      <c r="W6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X6" s="0" t="n">
+      <c r="W6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="Y6" s="2" t="b">
+      <c r="Y6" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="0" t="s">
+      <c r="Z6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AA6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AB6" s="0" t="s">
+      <c r="AB6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC6" s="0" t="s">
+      <c r="AC6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AI6" s="0" t="s">
+      <c r="AI6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ6" s="0" t="s">
+      <c r="AJ6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AK6" s="2" t="b">
+      <c r="AK6" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL6" s="0" t="s">
+      <c r="AL6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AM6" s="0" t="s">
+      <c r="AM6" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" customFormat="false" ht="2755.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>87.841651</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>2830</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>1818</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>1280</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>1408</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>80.515529</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7" s="1" t="n">
         <v>1685</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="1" t="n">
         <v>2035</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="1" t="n">
         <v>1792</v>
       </c>
-      <c r="O7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" s="0" t="s">
+      <c r="O7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="Q7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="R7" s="0" t="n">
+      <c r="R7" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="S7" s="0" t="n">
+      <c r="S7" s="1" t="n">
         <v>22.374571</v>
       </c>
-      <c r="T7" s="0" t="n">
+      <c r="T7" s="1" t="n">
         <v>13326</v>
       </c>
-      <c r="U7" s="0" t="n">
+      <c r="U7" s="1" t="n">
         <v>489</v>
       </c>
-      <c r="V7" s="0" t="n">
+      <c r="V7" s="1" t="n">
         <v>11136</v>
       </c>
-      <c r="W7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X7" s="0" t="n">
+      <c r="W7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="Y7" s="2" t="b">
+      <c r="Y7" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z7" s="0" t="s">
+      <c r="Z7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AA7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AB7" s="0" t="s">
+      <c r="AB7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AF7" s="0" t="s">
+      <c r="AF7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AG7" s="0" t="n">
+      <c r="AG7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AH7" s="0" t="n">
+      <c r="AH7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AI7" s="0" t="s">
+      <c r="AI7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ7" s="0" t="s">
+      <c r="AJ7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AK7" s="2" t="b">
+      <c r="AK7" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AL7" s="0" t="s">
+      <c r="AL7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AM7" s="0" t="s">
+      <c r="AM7" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="162.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>97.628854</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>2733</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>1607</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>960</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="G8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>88.056456</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8" s="1" t="n">
         <v>1788</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="M8" s="1" t="n">
         <v>1479</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="N8" s="1" t="n">
         <v>1216</v>
       </c>
-      <c r="O8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" s="0" t="s">
+      <c r="O8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="Q8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="R8" s="0" t="n">
+      <c r="R8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="S8" s="0" t="n">
+      <c r="S8" s="1" t="n">
         <v>8.543804</v>
       </c>
-      <c r="T8" s="0" t="n">
+      <c r="T8" s="1" t="n">
         <v>4342</v>
       </c>
-      <c r="U8" s="0" t="n">
+      <c r="U8" s="1" t="n">
         <v>428</v>
       </c>
-      <c r="V8" s="0" t="n">
+      <c r="V8" s="1" t="n">
         <v>2560</v>
       </c>
-      <c r="W8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X8" s="0" t="n">
+      <c r="W8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="Y8" s="2" t="b">
+      <c r="Y8" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z8" s="0" t="s">
+      <c r="Z8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AA8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AB8" s="0" t="s">
+      <c r="AB8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC8" s="0" t="s">
+      <c r="AC8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AI8" s="0" t="s">
+      <c r="AI8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ8" s="0" t="s">
+      <c r="AJ8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AK8" s="2" t="b">
+      <c r="AK8" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL8" s="0" t="s">
+      <c r="AL8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AM8" s="0" t="s">
+      <c r="AM8" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="176.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>82.885125</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>2908</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>1727</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>960</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>1408</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="1" t="n">
         <v>85.858758</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9" s="1" t="n">
         <v>1906</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M9" s="1" t="n">
         <v>1838</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N9" s="1" t="n">
         <v>1600</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="O9" s="1" t="n">
         <v>1536</v>
       </c>
-      <c r="P9" s="0" t="s">
+      <c r="P9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="Q9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="R9" s="0" t="n">
+      <c r="R9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S9" s="0" t="n">
+      <c r="S9" s="1" t="n">
         <v>6.700865</v>
       </c>
-      <c r="T9" s="0" t="n">
+      <c r="T9" s="1" t="n">
         <v>3618</v>
       </c>
-      <c r="U9" s="0" t="n">
+      <c r="U9" s="1" t="n">
         <v>337</v>
       </c>
-      <c r="V9" s="0" t="n">
+      <c r="V9" s="1" t="n">
         <v>1280</v>
       </c>
-      <c r="W9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X9" s="0" t="n">
+      <c r="W9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="Y9" s="2" t="b">
+      <c r="Y9" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z9" s="0" t="s">
+      <c r="Z9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AA9" s="1" t="s">
+      <c r="AA9" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="AB9" s="0" t="s">
+      <c r="AB9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AC9" s="0" t="s">
+      <c r="AC9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AI9" s="0" t="s">
+      <c r="AI9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ9" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK9" s="2" t="b">
+      <c r="AJ9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK9" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL9" s="0" t="s">
+      <c r="AL9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AM9" s="0" t="s">
+      <c r="AM9" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>79.44885</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>3616</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>1487</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>640</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="G10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="J10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10" s="1" t="n">
         <v>73.799416</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="L10" s="1" t="n">
         <v>1982</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="M10" s="1" t="n">
         <v>927</v>
       </c>
-      <c r="N10" s="0" t="n">
+      <c r="N10" s="1" t="n">
         <v>768</v>
       </c>
-      <c r="O10" s="0" t="n">
+      <c r="O10" s="1" t="n">
         <v>1664</v>
       </c>
-      <c r="P10" s="0" t="s">
+      <c r="P10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="Q10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="R10" s="0" t="n">
+      <c r="R10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="S10" s="0" t="n">
+      <c r="S10" s="1" t="n">
         <v>5.636065</v>
       </c>
-      <c r="T10" s="0" t="n">
+      <c r="T10" s="1" t="n">
         <v>3938</v>
       </c>
-      <c r="U10" s="0" t="n">
+      <c r="U10" s="1" t="n">
         <v>173</v>
       </c>
-      <c r="V10" s="0" t="n">
+      <c r="V10" s="1" t="n">
         <v>1280</v>
       </c>
-      <c r="W10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X10" s="0" t="n">
+      <c r="W10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Y10" s="2" t="b">
+      <c r="Y10" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z10" s="0" t="s">
+      <c r="Z10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AA10" s="0" t="s">
+      <c r="AA10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AB10" s="0" t="s">
+      <c r="AB10" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AI10" s="0" t="s">
+      <c r="AI10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AJ10" s="0" t="s">
+      <c r="AJ10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AK10" s="2" t="b">
+      <c r="AK10" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL10" s="0" t="s">
+      <c r="AL10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM10" s="0" t="s">
+      <c r="AM10" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="305.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>79.142859</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>2797</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>1727</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>704</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="G11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="J11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="1" t="n">
         <v>117.829347</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11" s="1" t="n">
         <v>2152</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11" s="1" t="n">
         <v>1660</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="1" t="n">
         <v>1536</v>
       </c>
-      <c r="O11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" s="0" t="s">
+      <c r="O11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="Q11" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="R11" s="0" t="n">
+      <c r="R11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S11" s="0" t="n">
+      <c r="S11" s="1" t="n">
         <v>16.000363</v>
       </c>
-      <c r="T11" s="0" t="n">
+      <c r="T11" s="1" t="n">
         <v>2746</v>
       </c>
-      <c r="U11" s="0" t="n">
+      <c r="U11" s="1" t="n">
         <v>439</v>
       </c>
-      <c r="V11" s="0" t="n">
+      <c r="V11" s="1" t="n">
         <v>1152</v>
       </c>
-      <c r="W11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X11" s="0" t="n">
+      <c r="W11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="Y11" s="2" t="b">
+      <c r="Y11" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z11" s="0" t="s">
+      <c r="Z11" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AA11" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AC11" s="0" t="s">
+      <c r="AC11" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AE11" s="0" t="s">
+      <c r="AE11" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AI11" s="0" t="s">
+      <c r="AI11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ11" s="0" t="s">
+      <c r="AJ11" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AK11" s="2" t="b">
+      <c r="AK11" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL11" s="0" t="s">
+      <c r="AL11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AM11" s="0" t="s">
+      <c r="AM11" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="86.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>27.974503</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>3295</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>1802</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>640</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>1792</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="J12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="1" t="n">
         <v>74.992223</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12" s="1" t="n">
         <v>2287</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M12" s="1" t="n">
         <v>1445</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N12" s="1" t="n">
         <v>1280</v>
       </c>
-      <c r="O12" s="0" t="n">
+      <c r="O12" s="1" t="n">
         <v>1408</v>
       </c>
-      <c r="P12" s="0" t="s">
+      <c r="P12" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="Q12" s="0" t="s">
+      <c r="Q12" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="R12" s="0" t="n">
+      <c r="R12" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="S12" s="0" t="n">
+      <c r="S12" s="1" t="n">
         <v>6.155146</v>
       </c>
-      <c r="T12" s="0" t="n">
+      <c r="T12" s="1" t="n">
         <v>4594</v>
       </c>
-      <c r="U12" s="0" t="n">
+      <c r="U12" s="1" t="n">
         <v>216</v>
       </c>
-      <c r="V12" s="0" t="n">
+      <c r="V12" s="1" t="n">
         <v>2816</v>
       </c>
-      <c r="W12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X12" s="0" t="n">
+      <c r="W12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Y12" s="2" t="b">
+      <c r="Y12" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z12" s="1" t="s">
+      <c r="Z12" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA12" s="1" t="s">
+      <c r="AA12" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AB12" s="0" t="s">
+      <c r="AB12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AI12" s="0" t="s">
+      <c r="AI12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ12" s="0" t="s">
+      <c r="AJ12" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AK12" s="2" t="b">
+      <c r="AK12" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL12" s="0" t="s">
+      <c r="AL12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM12" s="0" t="s">
+      <c r="AM12" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="148.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>80.145286</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>3397</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>1831</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>640</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="J13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="1" t="n">
         <v>90.351</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13" s="1" t="n">
         <v>2314</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M13" s="1" t="n">
         <v>1784</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N13" s="1" t="n">
         <v>1664</v>
       </c>
-      <c r="O13" s="0" t="n">
+      <c r="O13" s="1" t="n">
         <v>1792</v>
       </c>
-      <c r="P13" s="0" t="s">
+      <c r="P13" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="Q13" s="0" t="s">
+      <c r="Q13" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="R13" s="0" t="n">
+      <c r="R13" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="S13" s="0" t="n">
+      <c r="S13" s="1" t="n">
         <v>8.748809</v>
       </c>
-      <c r="T13" s="0" t="n">
+      <c r="T13" s="1" t="n">
         <v>4568</v>
       </c>
-      <c r="U13" s="0" t="n">
+      <c r="U13" s="1" t="n">
         <v>380</v>
       </c>
-      <c r="V13" s="0" t="n">
+      <c r="V13" s="1" t="n">
         <v>2560</v>
       </c>
-      <c r="W13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X13" s="0" t="n">
+      <c r="W13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Y13" s="2" t="b">
+      <c r="Y13" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z13" s="0" t="s">
+      <c r="Z13" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AA13" s="1" t="s">
+      <c r="AA13" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AB13" s="0" t="s">
+      <c r="AB13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC13" s="0" t="s">
+      <c r="AC13" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AE13" s="0" t="s">
+      <c r="AE13" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AI13" s="0" t="s">
+      <c r="AI13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ13" s="0" t="s">
+      <c r="AJ13" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AK13" s="2" t="b">
+      <c r="AK13" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL13" s="0" t="s">
+      <c r="AL13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM13" s="0" t="s">
+      <c r="AM13" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="155.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>91.274005</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>3685</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>1999</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>640</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>1920</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="J14" s="0" t="s">
+      <c r="J14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="1" t="n">
         <v>77.588045</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="L14" s="1" t="n">
         <v>2476</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="M14" s="1" t="n">
         <v>1477</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="N14" s="1" t="n">
         <v>1344</v>
       </c>
-      <c r="O14" s="0" t="n">
+      <c r="O14" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="P14" s="0" t="s">
+      <c r="P14" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="Q14" s="0" t="s">
+      <c r="Q14" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="R14" s="0" t="n">
+      <c r="R14" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="S14" s="0" t="n">
+      <c r="S14" s="1" t="n">
         <v>25.160623</v>
       </c>
-      <c r="T14" s="0" t="n">
+      <c r="T14" s="1" t="n">
         <v>29485</v>
       </c>
-      <c r="U14" s="0" t="n">
+      <c r="U14" s="1" t="n">
         <v>725</v>
       </c>
-      <c r="V14" s="0" t="n">
+      <c r="V14" s="1" t="n">
         <v>19840</v>
       </c>
-      <c r="W14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X14" s="0" t="n">
+      <c r="W14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="Y14" s="2" t="b">
+      <c r="Y14" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="Z14" s="1" t="s">
+      <c r="Z14" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AA14" s="1" t="s">
+      <c r="AA14" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="AB14" s="0" t="s">
+      <c r="AB14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC14" s="0" t="s">
+      <c r="AC14" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AI14" s="0" t="s">
+      <c r="AI14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AJ14" s="0" t="s">
+      <c r="AJ14" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AK14" s="2" t="b">
+      <c r="AK14" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AL14" s="0" t="s">
+      <c r="AL14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM14" s="0" t="s">
+      <c r="AM14" s="1" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="160.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>97.405995</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>6624</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>3042</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>1472</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>2304</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="J15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="1" t="n">
         <v>84.563405</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15" s="1" t="n">
         <v>2677</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15" s="1" t="n">
         <v>1204</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="N15" s="1" t="n">
         <v>1024</v>
       </c>
-      <c r="O15" s="0" t="n">
+      <c r="O15" s="1" t="n">
         <v>2176</v>
       </c>
-      <c r="P15" s="0" t="s">
+      <c r="P15" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="Q15" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="R15" s="0" t="n">
+      <c r="R15" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="S15" s="0" t="n">
+      <c r="S15" s="1" t="n">
         <v>17.880102</v>
       </c>
-      <c r="T15" s="0" t="n">
+      <c r="T15" s="1" t="n">
         <v>20123</v>
       </c>
-      <c r="U15" s="0" t="n">
+      <c r="U15" s="1" t="n">
         <v>793</v>
       </c>
-      <c r="V15" s="0" t="n">
+      <c r="V15" s="1" t="n">
         <v>13952</v>
       </c>
-      <c r="W15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X15" s="0" t="n">
+      <c r="W15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="Y15" s="2" t="b">
+      <c r="Y15" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z15" s="1" t="s">
+      <c r="Z15" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="AA15" s="1" t="s">
+      <c r="AA15" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="AB15" s="0" t="s">
+      <c r="AB15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC15" s="0" t="s">
+      <c r="AC15" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AE15" s="0" t="s">
+      <c r="AE15" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AI15" s="0" t="s">
+      <c r="AI15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AJ15" s="0" t="s">
+      <c r="AJ15" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AK15" s="2" t="b">
+      <c r="AK15" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL15" s="0" t="s">
+      <c r="AL15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AM15" s="0" t="s">
+      <c r="AM15" s="1" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>97.345078</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>8092</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>2749</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>1088</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>1792</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J16" s="0" t="s">
+      <c r="J16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="K16" s="1" t="n">
         <v>99.590723</v>
       </c>
-      <c r="L16" s="0" t="n">
+      <c r="L16" s="1" t="n">
         <v>2764</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="M16" s="1" t="n">
         <v>3161</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="N16" s="1" t="n">
         <v>3008</v>
       </c>
-      <c r="O16" s="0" t="n">
+      <c r="O16" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="P16" s="0" t="s">
+      <c r="P16" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="Q16" s="0" t="s">
+      <c r="Q16" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="R16" s="0" t="n">
+      <c r="R16" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="S16" s="0" t="n">
+      <c r="S16" s="1" t="n">
         <v>27.370885</v>
       </c>
-      <c r="T16" s="0" t="n">
+      <c r="T16" s="1" t="n">
         <v>15595</v>
       </c>
-      <c r="U16" s="0" t="n">
+      <c r="U16" s="1" t="n">
         <v>931</v>
       </c>
-      <c r="V16" s="0" t="n">
+      <c r="V16" s="1" t="n">
         <v>11904</v>
       </c>
-      <c r="W16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X16" s="0" t="n">
+      <c r="W16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X16" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="Y16" s="2" t="b">
+      <c r="Y16" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z16" s="1" t="s">
+      <c r="Z16" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="AA16" s="1" t="s">
+      <c r="AA16" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="AB16" s="0" t="s">
+      <c r="AB16" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="AC16" s="0" t="s">
+      <c r="AC16" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="AE16" s="0" t="s">
+      <c r="AE16" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="AF16" s="0" t="s">
+      <c r="AF16" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AI16" s="0" t="s">
+      <c r="AI16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ16" s="0" t="s">
+      <c r="AJ16" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="AK16" s="2" t="b">
+      <c r="AK16" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AL16" s="0" t="s">
+      <c r="AL16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AM16" s="0" t="s">
+      <c r="AM16" s="1" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>37.855121</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>5791</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>2893</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>960</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>2176</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="I17" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="J17" s="0" t="s">
+      <c r="J17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="K17" s="1" t="n">
         <v>93.063587</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="L17" s="1" t="n">
         <v>3026</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="M17" s="1" t="n">
         <v>2802</v>
       </c>
-      <c r="N17" s="0" t="n">
+      <c r="N17" s="1" t="n">
         <v>2624</v>
       </c>
-      <c r="O17" s="0" t="n">
+      <c r="O17" s="1" t="n">
         <v>1792</v>
       </c>
-      <c r="P17" s="0" t="s">
+      <c r="P17" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="Q17" s="0" t="s">
+      <c r="Q17" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="R17" s="0" t="n">
+      <c r="R17" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S17" s="0" t="n">
+      <c r="S17" s="1" t="n">
         <v>7.290256</v>
       </c>
-      <c r="T17" s="0" t="n">
+      <c r="T17" s="1" t="n">
         <v>2948</v>
       </c>
-      <c r="U17" s="0" t="n">
+      <c r="U17" s="1" t="n">
         <v>341</v>
       </c>
-      <c r="V17" s="0" t="n">
+      <c r="V17" s="1" t="n">
         <v>1152</v>
       </c>
-      <c r="W17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X17" s="0" t="n">
+      <c r="W17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X17" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Y17" s="2" t="b">
+      <c r="Y17" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z17" s="0" t="s">
+      <c r="Z17" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="AA17" s="1" t="s">
+      <c r="AA17" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="AB17" s="0" t="s">
+      <c r="AB17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AF17" s="0" t="s">
+      <c r="AF17" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AI17" s="0" t="s">
+      <c r="AI17" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AJ17" s="0" t="s">
+      <c r="AJ17" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="AK17" s="2" t="b">
+      <c r="AK17" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AL17" s="0" t="s">
+      <c r="AL17" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="AM17" s="0" t="s">
+      <c r="AM17" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>61.291548</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>4230</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>3332</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>1280</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>2816</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="I18" s="0" t="s">
+      <c r="I18" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="J18" s="0" t="s">
+      <c r="J18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="K18" s="1" t="n">
         <v>20.71158</v>
       </c>
-      <c r="L18" s="0" t="n">
+      <c r="L18" s="1" t="n">
         <v>3138</v>
       </c>
-      <c r="M18" s="0" t="n">
+      <c r="M18" s="1" t="n">
         <v>1539</v>
       </c>
-      <c r="N18" s="0" t="n">
+      <c r="N18" s="1" t="n">
         <v>1344</v>
       </c>
-      <c r="O18" s="0" t="n">
+      <c r="O18" s="1" t="n">
         <v>2432</v>
       </c>
-      <c r="P18" s="0" t="s">
+      <c r="P18" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="Q18" s="0" t="s">
+      <c r="Q18" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="R18" s="0" t="n">
+      <c r="R18" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="S18" s="0" t="n">
+      <c r="S18" s="1" t="n">
         <v>29.179208</v>
       </c>
-      <c r="T18" s="0" t="n">
+      <c r="T18" s="1" t="n">
         <v>8726</v>
       </c>
-      <c r="U18" s="0" t="n">
+      <c r="U18" s="1" t="n">
         <v>996</v>
       </c>
-      <c r="V18" s="0" t="n">
+      <c r="V18" s="1" t="n">
         <v>5888</v>
       </c>
-      <c r="W18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X18" s="0" t="n">
+      <c r="W18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X18" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="Y18" s="2" t="b">
+      <c r="Y18" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z18" s="0" t="s">
+      <c r="Z18" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="AA18" s="1" t="s">
+      <c r="AA18" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="AB18" s="0" t="s">
+      <c r="AB18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AF18" s="0" t="s">
+      <c r="AF18" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AH18" s="0" t="n">
+      <c r="AH18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AI18" s="0" t="s">
+      <c r="AI18" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AJ18" s="0" t="s">
+      <c r="AJ18" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="AK18" s="2" t="b">
+      <c r="AK18" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AL18" s="0" t="s">
+      <c r="AL18" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AM18" s="0" t="s">
+      <c r="AM18" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>40.985613</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>5495</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>3282</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>1152</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>2688</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="I19" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="J19" s="0" t="s">
+      <c r="J19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="K19" s="1" t="n">
         <v>84.588359</v>
       </c>
-      <c r="L19" s="0" t="n">
+      <c r="L19" s="1" t="n">
         <v>3214</v>
       </c>
-      <c r="M19" s="0" t="n">
+      <c r="M19" s="1" t="n">
         <v>1881</v>
       </c>
-      <c r="N19" s="0" t="n">
+      <c r="N19" s="1" t="n">
         <v>1600</v>
       </c>
-      <c r="O19" s="0" t="n">
+      <c r="O19" s="1" t="n">
         <v>2816</v>
       </c>
-      <c r="P19" s="0" t="s">
+      <c r="P19" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="Q19" s="0" t="s">
+      <c r="Q19" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="R19" s="0" t="n">
+      <c r="R19" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S19" s="0" t="n">
+      <c r="S19" s="1" t="n">
         <v>7.090414</v>
       </c>
-      <c r="T19" s="0" t="n">
+      <c r="T19" s="1" t="n">
         <v>2949</v>
       </c>
-      <c r="U19" s="0" t="n">
+      <c r="U19" s="1" t="n">
         <v>383</v>
       </c>
-      <c r="V19" s="0" t="n">
+      <c r="V19" s="1" t="n">
         <v>1408</v>
       </c>
-      <c r="W19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X19" s="0" t="n">
+      <c r="W19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X19" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="Y19" s="2" t="b">
+      <c r="Y19" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z19" s="1" t="s">
+      <c r="Z19" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AA19" s="1" t="s">
+      <c r="AA19" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="AB19" s="0" t="s">
+      <c r="AB19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AF19" s="0" t="s">
+      <c r="AF19" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AH19" s="0" t="n">
+      <c r="AH19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AI19" s="0" t="s">
+      <c r="AI19" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AJ19" s="0" t="s">
+      <c r="AJ19" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="AK19" s="2" t="b">
+      <c r="AK19" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AL19" s="0" t="s">
+      <c r="AL19" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AM19" s="0" t="s">
+      <c r="AM19" s="1" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>54.356967</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>4298</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>2833</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <v>768</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="1" t="n">
         <v>3072</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="I20" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="J20" s="0" t="s">
+      <c r="J20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="K20" s="1" t="n">
         <v>86.51938</v>
       </c>
-      <c r="L20" s="0" t="n">
+      <c r="L20" s="1" t="n">
         <v>3148</v>
       </c>
-      <c r="M20" s="0" t="n">
+      <c r="M20" s="1" t="n">
         <v>2737</v>
       </c>
-      <c r="N20" s="0" t="n">
+      <c r="N20" s="1" t="n">
         <v>2496</v>
       </c>
-      <c r="O20" s="0" t="n">
+      <c r="O20" s="1" t="n">
         <v>1408</v>
       </c>
-      <c r="P20" s="0" t="s">
+      <c r="P20" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="Q20" s="0" t="s">
+      <c r="Q20" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="R20" s="0" t="n">
+      <c r="R20" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="S20" s="0" t="n">
+      <c r="S20" s="1" t="n">
         <v>48.867135</v>
       </c>
-      <c r="T20" s="0" t="n">
+      <c r="T20" s="1" t="n">
         <v>25147</v>
       </c>
-      <c r="U20" s="0" t="n">
+      <c r="U20" s="1" t="n">
         <v>1731</v>
       </c>
-      <c r="V20" s="0" t="n">
+      <c r="V20" s="1" t="n">
         <v>16256</v>
       </c>
-      <c r="W20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X20" s="0" t="n">
+      <c r="W20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="Y20" s="2" t="b">
+      <c r="Y20" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="Z20" s="1" t="s">
+      <c r="Z20" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="AA20" s="1" t="s">
+      <c r="AA20" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="AB20" s="0" t="s">
+      <c r="AB20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC20" s="0" t="s">
+      <c r="AC20" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="AE20" s="0" t="s">
+      <c r="AE20" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AF20" s="0" t="s">
+      <c r="AF20" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AI20" s="0" t="s">
+      <c r="AI20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ20" s="5" t="s">
+      <c r="AJ20" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="AK20" s="2" t="b">
+      <c r="AK20" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AL20" s="0" t="s">
+      <c r="AL20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AM20" s="0" t="s">
+      <c r="AM20" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>32.127748</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>6556</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>3643</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <v>1408</v>
       </c>
-      <c r="G21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1" t="s">
+      <c r="G21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="J21" s="0" t="s">
+      <c r="J21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="K21" s="1" t="n">
         <v>74.156236</v>
       </c>
-      <c r="L21" s="0" t="n">
+      <c r="L21" s="1" t="n">
         <v>3311</v>
       </c>
-      <c r="M21" s="0" t="n">
+      <c r="M21" s="1" t="n">
         <v>1554</v>
       </c>
-      <c r="N21" s="0" t="n">
+      <c r="N21" s="1" t="n">
         <v>1408</v>
       </c>
-      <c r="O21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P21" s="0" t="s">
+      <c r="O21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="Q21" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="R21" s="0" t="n">
+      <c r="R21" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S21" s="0" t="n">
+      <c r="S21" s="1" t="n">
         <v>5.899153</v>
       </c>
-      <c r="T21" s="0" t="n">
+      <c r="T21" s="1" t="n">
         <v>2724</v>
       </c>
-      <c r="U21" s="0" t="n">
+      <c r="U21" s="1" t="n">
         <v>266</v>
       </c>
-      <c r="V21" s="0" t="n">
+      <c r="V21" s="1" t="n">
         <v>1152</v>
       </c>
-      <c r="W21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X21" s="0" t="n">
+      <c r="W21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Y21" s="2" t="b">
+      <c r="Y21" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z21" s="0" t="s">
+      <c r="Z21" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="AA21" s="1" t="s">
+      <c r="AA21" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="AB21" s="0" t="s">
+      <c r="AB21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC21" s="0" t="s">
+      <c r="AC21" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="AD21" s="0" t="s">
+      <c r="AD21" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="AI21" s="0" t="s">
+      <c r="AI21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AJ21" s="0" t="s">
+      <c r="AJ21" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="AK21" s="2" t="b">
+      <c r="AK21" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL21" s="0" t="s">
+      <c r="AL21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM21" s="0" t="s">
+      <c r="AM21" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>105.126811</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>4357</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>3342</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="1" t="n">
         <v>832</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="1" t="n">
         <v>1664</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="I22" s="0" t="s">
+      <c r="I22" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J22" s="0" t="s">
+      <c r="J22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="K22" s="1" t="n">
         <v>79.646935</v>
       </c>
-      <c r="L22" s="0" t="n">
+      <c r="L22" s="1" t="n">
         <v>3573</v>
       </c>
-      <c r="M22" s="0" t="n">
+      <c r="M22" s="1" t="n">
         <v>1409</v>
       </c>
-      <c r="N22" s="0" t="n">
+      <c r="N22" s="1" t="n">
         <v>1152</v>
       </c>
-      <c r="O22" s="0" t="n">
+      <c r="O22" s="1" t="n">
         <v>2816</v>
       </c>
-      <c r="P22" s="0" t="s">
+      <c r="P22" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="Q22" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="R22" s="0" t="n">
+      <c r="R22" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="S22" s="0" t="n">
+      <c r="S22" s="1" t="n">
         <v>4.289916</v>
       </c>
-      <c r="T22" s="0" t="n">
+      <c r="T22" s="1" t="n">
         <v>4197</v>
       </c>
-      <c r="U22" s="0" t="n">
+      <c r="U22" s="1" t="n">
         <v>208</v>
       </c>
-      <c r="V22" s="0" t="n">
+      <c r="V22" s="1" t="n">
         <v>2560</v>
       </c>
-      <c r="W22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X22" s="0" t="n">
+      <c r="W22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X22" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Y22" s="2" t="b">
+      <c r="Y22" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z22" s="0" t="s">
+      <c r="Z22" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="AA22" s="1" t="s">
+      <c r="AA22" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="AB22" s="0" t="s">
+      <c r="AB22" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="AI22" s="0" t="s">
+      <c r="AI22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AJ22" s="0" t="s">
+      <c r="AJ22" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="AK22" s="2" t="b">
+      <c r="AK22" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL22" s="0" t="s">
+      <c r="AL22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM22" s="0" t="s">
+      <c r="AM22" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>88.402888</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>4467</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>3499</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="1" t="n">
         <v>768</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1" t="s">
+      <c r="G23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="I23" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="J23" s="0" t="s">
+      <c r="J23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="K23" s="1" t="n">
         <v>86.204755</v>
       </c>
-      <c r="L23" s="0" t="n">
+      <c r="L23" s="1" t="n">
         <v>3784</v>
       </c>
-      <c r="M23" s="0" t="n">
+      <c r="M23" s="1" t="n">
         <v>1668</v>
       </c>
-      <c r="N23" s="0" t="n">
+      <c r="N23" s="1" t="n">
         <v>1472</v>
       </c>
-      <c r="O23" s="0" t="n">
+      <c r="O23" s="1" t="n">
         <v>1408</v>
       </c>
-      <c r="P23" s="0" t="s">
+      <c r="P23" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="Q23" s="0" t="s">
+      <c r="Q23" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="R23" s="0" t="n">
+      <c r="R23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S23" s="0" t="n">
+      <c r="S23" s="1" t="n">
         <v>13.675129</v>
       </c>
-      <c r="T23" s="0" t="n">
+      <c r="T23" s="1" t="n">
         <v>4110</v>
       </c>
-      <c r="U23" s="0" t="n">
+      <c r="U23" s="1" t="n">
         <v>494</v>
       </c>
-      <c r="V23" s="0" t="n">
+      <c r="V23" s="1" t="n">
         <v>1280</v>
       </c>
-      <c r="W23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X23" s="0" t="n">
+      <c r="W23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Y23" s="2" t="b">
+      <c r="Y23" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z23" s="0" t="s">
+      <c r="Z23" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AA23" s="1" t="s">
+      <c r="AA23" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="AB23" s="0" t="s">
+      <c r="AB23" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="AC23" s="0" t="s">
+      <c r="AC23" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AD23" s="0" t="s">
+      <c r="AD23" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AI23" s="0" t="s">
+      <c r="AI23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AJ23" s="0" t="s">
+      <c r="AJ23" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="AK23" s="2" t="b">
+      <c r="AK23" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL23" s="0" t="s">
+      <c r="AL23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM23" s="0" t="s">
+      <c r="AM23" s="1" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>118.572771</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <v>6074</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>4410</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="1" t="n">
         <v>1536</v>
       </c>
-      <c r="G24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1" t="s">
+      <c r="G24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="I24" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="J24" s="0" t="s">
+      <c r="J24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="K24" s="1" t="n">
         <v>81.38857</v>
       </c>
-      <c r="L24" s="0" t="n">
+      <c r="L24" s="1" t="n">
         <v>3920</v>
       </c>
-      <c r="M24" s="0" t="n">
+      <c r="M24" s="1" t="n">
         <v>2088</v>
       </c>
-      <c r="N24" s="0" t="n">
+      <c r="N24" s="1" t="n">
         <v>1920</v>
       </c>
-      <c r="O24" s="0" t="n">
+      <c r="O24" s="1" t="n">
         <v>3328</v>
       </c>
-      <c r="P24" s="0" t="s">
+      <c r="P24" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="Q24" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="R24" s="0" t="n">
+      <c r="R24" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S24" s="0" t="n">
+      <c r="S24" s="1" t="n">
         <v>4.318085</v>
       </c>
-      <c r="T24" s="0" t="n">
+      <c r="T24" s="1" t="n">
         <v>2401</v>
       </c>
-      <c r="U24" s="0" t="n">
+      <c r="U24" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="V24" s="0" t="n">
+      <c r="V24" s="1" t="n">
         <v>1152</v>
       </c>
-      <c r="W24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X24" s="0" t="n">
+      <c r="W24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Y24" s="2" t="b">
+      <c r="Y24" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z24" s="0" t="s">
+      <c r="Z24" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="AA24" s="0" t="s">
+      <c r="AA24" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="AB24" s="0" t="s">
+      <c r="AB24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AI24" s="0" t="s">
+      <c r="AI24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ24" s="0" t="s">
+      <c r="AJ24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AK24" s="2" t="b">
+      <c r="AK24" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AL24" s="0" t="s">
+      <c r="AL24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM24" s="0" t="s">
+      <c r="AM24" s="1" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>99.088729</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>4518</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>3979</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="1" t="n">
         <v>1024</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <v>3712</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="I25" s="0" t="s">
+      <c r="I25" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="J25" s="0" t="s">
+      <c r="J25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="K25" s="1" t="n">
         <v>84.464894</v>
       </c>
-      <c r="L25" s="0" t="n">
+      <c r="L25" s="1" t="n">
         <v>4001</v>
       </c>
-      <c r="M25" s="0" t="n">
+      <c r="M25" s="1" t="n">
         <v>1894</v>
       </c>
-      <c r="N25" s="0" t="n">
+      <c r="N25" s="1" t="n">
         <v>1728</v>
       </c>
-      <c r="O25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P25" s="0" t="s">
+      <c r="O25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="Q25" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="R25" s="0" t="n">
+      <c r="R25" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="S25" s="0" t="n">
+      <c r="S25" s="1" t="n">
         <v>8.617238</v>
       </c>
-      <c r="T25" s="0" t="n">
+      <c r="T25" s="1" t="n">
         <v>3760</v>
       </c>
-      <c r="U25" s="0" t="n">
+      <c r="U25" s="1" t="n">
         <v>301</v>
       </c>
-      <c r="V25" s="0" t="n">
+      <c r="V25" s="1" t="n">
         <v>2304</v>
       </c>
-      <c r="W25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X25" s="0" t="n">
+      <c r="W25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X25" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Y25" s="2" t="b">
+      <c r="Y25" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z25" s="0" t="s">
+      <c r="Z25" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="AA25" s="1" t="s">
+      <c r="AA25" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="AB25" s="0" t="s">
+      <c r="AB25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AI25" s="0" t="s">
+      <c r="AI25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ25" s="0" t="s">
+      <c r="AJ25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AK25" s="2" t="b">
+      <c r="AK25" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AL25" s="0" t="s">
+      <c r="AL25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM25" s="0" t="s">
+      <c r="AM25" s="1" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>98.081067</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>4782</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>4393</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="1" t="n">
         <v>1216</v>
       </c>
-      <c r="G26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1" t="s">
+      <c r="G26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="I26" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="J26" s="0" t="s">
+      <c r="J26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K26" s="0" t="n">
+      <c r="K26" s="1" t="n">
         <v>77.733598</v>
       </c>
-      <c r="L26" s="0" t="n">
+      <c r="L26" s="1" t="n">
         <v>4216</v>
       </c>
-      <c r="M26" s="0" t="n">
+      <c r="M26" s="1" t="n">
         <v>1654</v>
       </c>
-      <c r="N26" s="0" t="n">
+      <c r="N26" s="1" t="n">
         <v>1408</v>
       </c>
-      <c r="O26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P26" s="0" t="s">
+      <c r="O26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="Q26" s="1" t="s">
+      <c r="Q26" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="R26" s="0" t="n">
+      <c r="R26" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S26" s="0" t="n">
+      <c r="S26" s="1" t="n">
         <v>4.416412</v>
       </c>
-      <c r="T26" s="0" t="n">
+      <c r="T26" s="1" t="n">
         <v>2557</v>
       </c>
-      <c r="U26" s="0" t="n">
+      <c r="U26" s="1" t="n">
         <v>154</v>
       </c>
-      <c r="V26" s="0" t="n">
+      <c r="V26" s="1" t="n">
         <v>1152</v>
       </c>
-      <c r="W26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X26" s="0" t="n">
+      <c r="W26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Y26" s="2" t="b">
+      <c r="Y26" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z26" s="0" t="s">
+      <c r="Z26" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="AA26" s="1" t="s">
+      <c r="AA26" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="AB26" s="0" t="s">
+      <c r="AB26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AI26" s="0" t="s">
+      <c r="AI26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ26" s="0" t="s">
+      <c r="AJ26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AK26" s="2" t="b">
+      <c r="AK26" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL26" s="0" t="s">
+      <c r="AL26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM26" s="0" t="s">
+      <c r="AM26" s="1" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>103.334711</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>4901</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>3984</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="1" t="n">
         <v>960</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="1" t="n">
         <v>3456</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="I27" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="J27" s="0" t="s">
+      <c r="J27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K27" s="0" t="n">
+      <c r="K27" s="1" t="n">
         <v>78.467044</v>
       </c>
-      <c r="L27" s="0" t="n">
+      <c r="L27" s="1" t="n">
         <v>4067</v>
       </c>
-      <c r="M27" s="0" t="n">
+      <c r="M27" s="1" t="n">
         <v>1891</v>
       </c>
-      <c r="N27" s="0" t="n">
+      <c r="N27" s="1" t="n">
         <v>1664</v>
       </c>
-      <c r="O27" s="0" t="n">
+      <c r="O27" s="1" t="n">
         <v>3584</v>
       </c>
-      <c r="P27" s="0" t="s">
+      <c r="P27" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="Q27" s="0" t="s">
+      <c r="Q27" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="R27" s="0" t="n">
+      <c r="R27" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="S27" s="0" t="n">
+      <c r="S27" s="1" t="n">
         <v>5.101619</v>
       </c>
-      <c r="T27" s="0" t="n">
+      <c r="T27" s="1" t="n">
         <v>4728</v>
       </c>
-      <c r="U27" s="0" t="n">
+      <c r="U27" s="1" t="n">
         <v>223</v>
       </c>
-      <c r="V27" s="0" t="n">
+      <c r="V27" s="1" t="n">
         <v>2688</v>
       </c>
-      <c r="W27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X27" s="0" t="n">
+      <c r="W27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X27" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Y27" s="2" t="b">
+      <c r="Y27" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z27" s="0" t="s">
+      <c r="Z27" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="AA27" s="1" t="s">
+      <c r="AA27" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="AB27" s="0" t="s">
+      <c r="AB27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC27" s="0" t="s">
+      <c r="AC27" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="AI27" s="0" t="s">
+      <c r="AI27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ27" s="0" t="s">
+      <c r="AJ27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AK27" s="2" t="b">
+      <c r="AK27" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AL27" s="0" t="s">
+      <c r="AL27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM27" s="0" t="s">
+      <c r="AM27" s="1" t="s">
         <v>249</v>
       </c>
     </row>

</xml_diff>